<commit_message>
Cleansed the Data Files of various faulty enteries.
Modified the adresses of the Data Files in IPython notebooks, to run on any unix based machine.
Rectified presentation and code faults.
Included missing packages.
</commit_message>
<xml_diff>
--- a/Player Database/Alessandro.xlsx
+++ b/Player Database/Alessandro.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="23">
   <si>
     <t xml:space="preserve">TEAM</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">WCQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Substitute</t>
   </si>
   <si>
     <t xml:space="preserve">Europa</t>
@@ -317,14 +314,13 @@
   </sheetPr>
   <dimension ref="A1:H483"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A234" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D254" activeCellId="0" sqref="D254 D256:D257 D260 D263 D455 D457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="14.1734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6707,8 +6703,8 @@
       <c r="C254" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D254" s="3" t="s">
-        <v>19</v>
+      <c r="D254" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="E254" s="3" t="n">
         <v>0</v>
@@ -6759,8 +6755,8 @@
       <c r="C256" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D256" s="3" t="s">
-        <v>19</v>
+      <c r="D256" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="E256" s="3" t="n">
         <v>0</v>
@@ -6785,8 +6781,8 @@
       <c r="C257" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D257" s="3" t="s">
-        <v>19</v>
+      <c r="D257" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="E257" s="3" t="n">
         <v>2</v>
@@ -6863,8 +6859,8 @@
       <c r="C260" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D260" s="3" t="s">
-        <v>19</v>
+      <c r="D260" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="E260" s="3" t="n">
         <v>0</v>
@@ -6941,8 +6937,8 @@
       <c r="C263" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D263" s="3" t="s">
-        <v>19</v>
+      <c r="D263" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="E263" s="3" t="n">
         <v>0</v>
@@ -8859,7 +8855,7 @@
         <v>40255</v>
       </c>
       <c r="C339" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D339" s="3" t="n">
         <v>6</v>
@@ -8911,7 +8907,7 @@
         <v>40248</v>
       </c>
       <c r="C341" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D341" s="3" t="n">
         <v>0</v>
@@ -8973,7 +8969,7 @@
         <v>40234</v>
       </c>
       <c r="C344" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D344" s="3" t="n">
         <v>85</v>
@@ -9025,7 +9021,7 @@
         <v>40227</v>
       </c>
       <c r="C346" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D346" s="3" t="n">
         <v>90</v>
@@ -10025,7 +10021,7 @@
         <v>40528</v>
       </c>
       <c r="C386" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D386" s="3" t="n">
         <v>90</v>
@@ -10103,7 +10099,7 @@
         <v>40513</v>
       </c>
       <c r="C389" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D389" s="3" t="n">
         <v>90</v>
@@ -10251,7 +10247,7 @@
         <v>40486</v>
       </c>
       <c r="C395" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D395" s="3" t="n">
         <v>90</v>
@@ -10329,7 +10325,7 @@
         <v>40472</v>
       </c>
       <c r="C398" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D398" s="3" t="n">
         <v>90</v>
@@ -10407,7 +10403,7 @@
         <v>40451</v>
       </c>
       <c r="C401" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D401" s="3" t="n">
         <v>90</v>
@@ -10511,7 +10507,7 @@
         <v>40437</v>
       </c>
       <c r="C405" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D405" s="3" t="n">
         <v>90</v>
@@ -10589,7 +10585,7 @@
         <v>40416</v>
       </c>
       <c r="C408" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D408" s="3" t="n">
         <v>90</v>
@@ -10615,7 +10611,7 @@
         <v>40409</v>
       </c>
       <c r="C409" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D409" s="3" t="n">
         <v>17</v>
@@ -10641,7 +10637,7 @@
         <v>40395</v>
       </c>
       <c r="C410" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D410" s="3" t="n">
         <v>44</v>
@@ -10667,7 +10663,7 @@
         <v>40388</v>
       </c>
       <c r="C411" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D411" s="3" t="n">
         <v>8</v>
@@ -11691,10 +11687,10 @@
         <v>40752</v>
       </c>
       <c r="C455" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D455" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="D455" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="E455" s="3" t="n">
         <v>0</v>
@@ -11717,7 +11713,7 @@
         <v>40750</v>
       </c>
       <c r="C456" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D456" s="3" t="n">
         <v>90</v>
@@ -11743,10 +11739,10 @@
         <v>40747</v>
       </c>
       <c r="C457" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D457" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="D457" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="E457" s="3" t="n">
         <v>1</v>
@@ -11763,13 +11759,13 @@
     </row>
     <row r="458" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B458" s="4" t="n">
         <v>41361</v>
       </c>
       <c r="C458" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D458" s="3" t="n">
         <v>90</v>
@@ -11789,13 +11785,13 @@
     </row>
     <row r="459" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B459" s="4" t="n">
         <v>41356</v>
       </c>
       <c r="C459" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D459" s="3" t="n">
         <v>90</v>
@@ -11815,13 +11811,13 @@
     </row>
     <row r="460" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B460" s="4" t="n">
         <v>41349</v>
       </c>
       <c r="C460" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D460" s="3" t="n">
         <v>90</v>
@@ -11841,13 +11837,13 @@
     </row>
     <row r="461" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B461" s="4" t="n">
         <v>41341</v>
       </c>
       <c r="C461" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D461" s="3" t="n">
         <v>90</v>
@@ -11867,13 +11863,13 @@
     </row>
     <row r="462" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B462" s="4" t="n">
         <v>41335</v>
       </c>
       <c r="C462" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D462" s="3" t="n">
         <v>90</v>
@@ -11893,13 +11889,13 @@
     </row>
     <row r="463" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B463" s="4" t="n">
         <v>41328</v>
       </c>
       <c r="C463" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D463" s="3" t="n">
         <v>90</v>
@@ -11919,13 +11915,13 @@
     </row>
     <row r="464" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B464" s="4" t="n">
         <v>41320</v>
       </c>
       <c r="C464" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D464" s="3" t="n">
         <v>90</v>
@@ -11945,13 +11941,13 @@
     </row>
     <row r="465" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B465" s="4" t="n">
         <v>41314</v>
       </c>
       <c r="C465" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D465" s="3" t="n">
         <v>90</v>
@@ -11971,13 +11967,13 @@
     </row>
     <row r="466" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B466" s="4" t="n">
         <v>41306</v>
       </c>
       <c r="C466" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D466" s="3" t="n">
         <v>90</v>
@@ -11997,13 +11993,13 @@
     </row>
     <row r="467" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B467" s="4" t="n">
         <v>41299</v>
       </c>
       <c r="C467" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D467" s="3" t="n">
         <v>90</v>
@@ -12023,13 +12019,13 @@
     </row>
     <row r="468" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B468" s="4" t="n">
         <v>41292</v>
       </c>
       <c r="C468" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D468" s="3" t="n">
         <v>82</v>
@@ -12049,13 +12045,13 @@
     </row>
     <row r="469" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B469" s="4" t="n">
         <v>41286</v>
       </c>
       <c r="C469" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D469" s="3" t="n">
         <v>90</v>
@@ -12075,13 +12071,13 @@
     </row>
     <row r="470" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B470" s="4" t="n">
         <v>41279</v>
       </c>
       <c r="C470" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D470" s="3" t="n">
         <v>90</v>
@@ -12101,13 +12097,13 @@
     </row>
     <row r="471" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B471" s="4" t="n">
         <v>41270</v>
       </c>
       <c r="C471" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D471" s="3" t="n">
         <v>90</v>
@@ -12127,13 +12123,13 @@
     </row>
     <row r="472" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B472" s="4" t="n">
         <v>41264</v>
       </c>
       <c r="C472" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D472" s="3" t="n">
         <v>90</v>
@@ -12153,13 +12149,13 @@
     </row>
     <row r="473" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B473" s="4" t="n">
         <v>41258</v>
       </c>
       <c r="C473" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D473" s="3" t="n">
         <v>20</v>
@@ -12179,13 +12175,13 @@
     </row>
     <row r="474" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B474" s="4" t="n">
         <v>41244</v>
       </c>
       <c r="C474" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D474" s="3" t="n">
         <v>68</v>
@@ -12205,13 +12201,13 @@
     </row>
     <row r="475" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B475" s="4" t="n">
         <v>41236</v>
       </c>
       <c r="C475" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D475" s="3" t="n">
         <v>90</v>
@@ -12231,13 +12227,13 @@
     </row>
     <row r="476" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B476" s="4" t="n">
         <v>41229</v>
       </c>
       <c r="C476" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D476" s="3" t="n">
         <v>90</v>
@@ -12257,13 +12253,13 @@
     </row>
     <row r="477" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B477" s="4" t="n">
         <v>41223</v>
       </c>
       <c r="C477" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D477" s="3" t="n">
         <v>63</v>
@@ -12283,13 +12279,13 @@
     </row>
     <row r="478" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B478" s="4" t="n">
         <v>41210</v>
       </c>
       <c r="C478" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D478" s="3" t="n">
         <v>90</v>
@@ -12309,13 +12305,13 @@
     </row>
     <row r="479" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B479" s="4" t="n">
         <v>41202</v>
       </c>
       <c r="C479" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D479" s="3" t="n">
         <v>90</v>
@@ -12335,13 +12331,13 @@
     </row>
     <row r="480" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B480" s="4" t="n">
         <v>41195</v>
       </c>
       <c r="C480" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D480" s="3" t="n">
         <v>90</v>
@@ -12361,13 +12357,13 @@
     </row>
     <row r="481" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B481" s="4" t="n">
         <v>41187</v>
       </c>
       <c r="C481" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D481" s="3" t="n">
         <v>90</v>
@@ -12387,13 +12383,13 @@
     </row>
     <row r="482" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B482" s="4" t="n">
         <v>41734</v>
       </c>
       <c r="C482" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D482" s="3" t="n">
         <v>90</v>
@@ -12413,13 +12409,13 @@
     </row>
     <row r="483" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B483" s="4" t="n">
         <v>41727</v>
       </c>
       <c r="C483" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D483" s="3" t="n">
         <v>90</v>

</xml_diff>